<commit_message>
se agrega la fila columna
</commit_message>
<xml_diff>
--- a/plantillas/cal20_consolidado.xlsx
+++ b/plantillas/cal20_consolidado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuar\Documents\Python Scripts\cal-analizador\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B4EFFB-40B1-4568-9923-712AD1A68901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A28BAF0-56D4-41E2-9349-D9CED38F5461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="110">
   <si>
     <t>Año</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>ARCHIVO</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -664,6 +667,60 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -676,10 +733,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -688,70 +748,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1036,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BP1" sqref="BP1:BP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1051,32 +1057,33 @@
     <col min="19" max="19" width="13.578125" customWidth="1"/>
     <col min="30" max="30" width="17.3125" customWidth="1"/>
     <col min="67" max="67" width="37.5234375" customWidth="1"/>
+    <col min="68" max="68" width="21.1015625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="34"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="27"/>
       <c r="P1" s="28" t="s">
         <v>4</v>
       </c>
@@ -1084,115 +1091,117 @@
       <c r="R1" s="29"/>
       <c r="S1" s="29"/>
       <c r="T1" s="30"/>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="13" t="s">
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="15" t="s">
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="17" t="s">
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
+      <c r="AW1" s="33"/>
+      <c r="AX1" s="33"/>
+      <c r="AY1" s="33"/>
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="17"/>
-      <c r="BF1" s="17"/>
-      <c r="BG1" s="17"/>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="18"/>
-      <c r="BP1" s="10"/>
+      <c r="BD1" s="41"/>
+      <c r="BE1" s="41"/>
+      <c r="BF1" s="41"/>
+      <c r="BG1" s="41"/>
+      <c r="BH1" s="41"/>
+      <c r="BI1" s="41"/>
+      <c r="BJ1" s="41"/>
+      <c r="BK1" s="41"/>
+      <c r="BL1" s="41"/>
+      <c r="BM1" s="41"/>
+      <c r="BN1" s="41"/>
+      <c r="BO1" s="42"/>
+      <c r="BP1" s="43" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="2" spans="1:68" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="26"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="24"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="19" t="s">
+      <c r="O2" s="37"/>
+      <c r="P2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="Q2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="19" t="s">
+      <c r="R2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="38" t="s">
         <v>14</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="22"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="21" t="s">
+      <c r="V2" s="36"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="21" t="s">
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="23"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="37"/>
       <c r="AD2" s="6"/>
-      <c r="AE2" s="37"/>
+      <c r="AE2" s="13"/>
       <c r="AF2" s="5"/>
       <c r="AG2" s="5"/>
       <c r="AH2" s="5"/>
@@ -1204,7 +1213,7 @@
       <c r="AN2" s="5"/>
       <c r="AO2" s="5"/>
       <c r="AP2" s="3"/>
-      <c r="AQ2" s="37"/>
+      <c r="AQ2" s="13"/>
       <c r="AR2" s="5"/>
       <c r="AS2" s="5"/>
       <c r="AT2" s="5"/>
@@ -1216,7 +1225,7 @@
       <c r="AZ2" s="5"/>
       <c r="BA2" s="5"/>
       <c r="BB2" s="3"/>
-      <c r="BC2" s="37"/>
+      <c r="BC2" s="13"/>
       <c r="BD2" s="5"/>
       <c r="BE2" s="5"/>
       <c r="BF2" s="5"/>
@@ -1229,12 +1238,12 @@
       <c r="BM2" s="5"/>
       <c r="BN2" s="5"/>
       <c r="BO2" s="3"/>
-      <c r="BP2" s="10"/>
+      <c r="BP2" s="23"/>
     </row>
     <row r="3" spans="1:68" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="26"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="24"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="2" t="s">
         <v>107</v>
       </c>
@@ -1263,10 +1272,10 @@
       <c r="O3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
       <c r="T3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1286,7 +1295,7 @@
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
       <c r="AD3" s="6"/>
-      <c r="AE3" s="38"/>
+      <c r="AE3" s="14"/>
       <c r="AF3" s="7" t="s">
         <v>28</v>
       </c>
@@ -1320,7 +1329,7 @@
       <c r="AP3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AQ3" s="38"/>
+      <c r="AQ3" s="14"/>
       <c r="AR3" s="7" t="s">
         <v>28</v>
       </c>
@@ -1354,7 +1363,7 @@
       <c r="BB3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="BC3" s="38"/>
+      <c r="BC3" s="14"/>
       <c r="BD3" s="7" t="s">
         <v>28</v>
       </c>
@@ -1391,12 +1400,12 @@
       <c r="BO3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="BP3" s="10"/>
+      <c r="BP3" s="23"/>
     </row>
     <row r="4" spans="1:68" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="2"/>
       <c r="E4" s="8" t="s">
         <v>40</v>
@@ -1419,10 +1428,10 @@
       <c r="O4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2" t="s">
         <v>42</v>
@@ -1440,7 +1449,7 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="9"/>
-      <c r="AE4" s="38"/>
+      <c r="AE4" s="14"/>
       <c r="AF4" s="7"/>
       <c r="AG4" s="7"/>
       <c r="AH4" s="7"/>
@@ -1452,7 +1461,7 @@
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
       <c r="AP4" s="2"/>
-      <c r="AQ4" s="38"/>
+      <c r="AQ4" s="14"/>
       <c r="AR4" s="7"/>
       <c r="AS4" s="7"/>
       <c r="AT4" s="7"/>
@@ -1464,7 +1473,7 @@
       <c r="AZ4" s="7"/>
       <c r="BA4" s="7"/>
       <c r="BB4" s="2"/>
-      <c r="BC4" s="38"/>
+      <c r="BC4" s="14"/>
       <c r="BD4" s="7"/>
       <c r="BE4" s="7"/>
       <c r="BF4" s="7"/>
@@ -1477,10 +1486,11 @@
       <c r="BM4" s="7"/>
       <c r="BN4" s="7"/>
       <c r="BO4" s="2"/>
+      <c r="BP4" s="23"/>
     </row>
     <row r="5" spans="1:68" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11"/>
-      <c r="B5" s="42"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="11" t="s">
         <v>43</v>
       </c>
@@ -1674,14 +1684,12 @@
       <c r="BO5" s="11" t="s">
         <v>106</v>
       </c>
+      <c r="BP5" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="P1:T1"/>
+  <mergeCells count="19">
+    <mergeCell ref="BC1:BO1"/>
+    <mergeCell ref="BP1:BP5"/>
     <mergeCell ref="AE1:AP1"/>
     <mergeCell ref="AQ1:BB1"/>
     <mergeCell ref="E2:G2"/>
@@ -1694,7 +1702,11 @@
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
     <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="BC1:BO1"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="P1:T1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ubicación (UTM) referenciada a la zona 17" sqref="E2:G4" xr:uid="{1EDCE92E-2671-49BA-B0B5-20D3B5729DD2}"/>

</xml_diff>